<commit_message>
Added many sensors to code, datasheets
</commit_message>
<xml_diff>
--- a/Hardware Information/Hardware Description.xlsx
+++ b/Hardware Information/Hardware Description.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="460" windowWidth="19200" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pin List" sheetId="1" r:id="rId1"/>
@@ -120,9 +120,6 @@
     <t>MLX90614; SHT21; ADS1015; BMP280</t>
   </si>
   <si>
-    <t>Board Voltage Divider</t>
-  </si>
-  <si>
     <t>Board LED, Red LED</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Davis Wind Speed</t>
+  </si>
+  <si>
+    <t>Feather Board Voltage Divider</t>
   </si>
 </sst>
 </file>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,7 +533,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -607,7 +607,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -631,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -639,7 +639,7 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>